<commit_message>
Removed redundant addition of <<index>> to pathes
</commit_message>
<xml_diff>
--- a/0_NotesAndTesting/Test und Beispiele Indexe/Variante2_ExampleCSV.xlsx
+++ b/0_NotesAndTesting/Test und Beispiele Indexe/Variante2_ExampleCSV.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B4D19A-63E4-4598-A3D1-490E0FE394CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610C1C17-7181-4422-876F-71C76BCA0D21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -209,6 +209,30 @@
   </si>
   <si>
     <t>Können wir die CSV-Struktur aus den Pfade erstellen und das ganze dann relativ leicht aus einer SQL-DB befüllen lassen? (Händische Mapping-Tabelle fiele weg, aber die Daten müssen korrekt in die CSV kommen</t>
+  </si>
+  <si>
+    <t>WENN die meisten Templates nur einen INDEX enthalten pro Pfad, dann ist das Problem der händischen Arbeit weniger groß</t>
+  </si>
+  <si>
+    <t>Jendrik prüft das in CKM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idee: Siehe Beispieltabelle oben. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oder </t>
+  </si>
+  <si>
+    <t>Spalten und Index-Spalten auslesen aus Template und dann korrekt befüllen lassen..kompliziert da mehr ETL?</t>
+  </si>
+  <si>
+    <t>CSV aus Daten z.B. SQL-DB erstellen -&gt; CSV-Spalten mappen auf Template, Index-Spalten hinzufügen soviele wie notwendig und befüllen (lassen?)</t>
+  </si>
+  <si>
+    <t>Wie aufwändig ist es die Index-Spalten automatisiert zu befüllen?</t>
+  </si>
+  <si>
+    <t>Indexe haben wir in den Pfaden da brauchen wir keine Abfrage auf CMD-Line..</t>
   </si>
 </sst>
 </file>
@@ -578,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,6 +1017,54 @@
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
     </row>
+    <row r="51" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C51" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C52" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="54" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>65</v>
+      </c>
+      <c r="F54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="L55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated notes about issue 18
</commit_message>
<xml_diff>
--- a/0_NotesAndTesting/Test und Beispiele Indexe/Variante2_ExampleCSV.xlsx
+++ b/0_NotesAndTesting/Test und Beispiele Indexe/Variante2_ExampleCSV.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610C1C17-7181-4422-876F-71C76BCA0D21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3FF694-227C-4BA1-82FB-54F1FF4C4AA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -233,6 +233,30 @@
   </si>
   <si>
     <t>Indexe haben wir in den Pfaden da brauchen wir keine Abfrage auf CMD-Line..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idee: </t>
+  </si>
+  <si>
+    <t>Wir reichern die bestehende CSV um die Index-Spalten an und lassen die durch den ETLer befüllen auf Basis der Ids bzw. einer Zuordnung zu einem Patienten/Ressource</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt; Die mappen CSVs auf unique FLAT Paths (sprich so wie wir am Anfang)</t>
+  </si>
+  <si>
+    <t>Das ist elegant um viele Einträge reinzuladen…</t>
+  </si>
+  <si>
+    <t>Siehe Beispiel Basketballer Injuries..</t>
+  </si>
+  <si>
+    <t>ERGEBNIS</t>
+  </si>
+  <si>
+    <t>Indexe sind nicht so häufig.</t>
+  </si>
+  <si>
+    <t>Einfach CSV_Spalten auf Pfade mappen und wenn nötig Index dazu angeben</t>
   </si>
 </sst>
 </file>
@@ -602,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,15 +887,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>49</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G19" s="5" t="s">
         <v>46</v>
       </c>
@@ -882,7 +909,7 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="2:13" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:15" ht="26.25" x14ac:dyDescent="0.4">
       <c r="E20" s="3" t="s">
         <v>18</v>
       </c>
@@ -896,29 +923,29 @@
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F25" s="2" t="s">
         <v>28</v>
       </c>
@@ -926,12 +953,12 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F28" s="2" t="s">
         <v>23</v>
       </c>
@@ -939,17 +966,17 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
         <v>34</v>
       </c>
@@ -1065,6 +1092,39 @@
         <v>67</v>
       </c>
     </row>
+    <row r="59" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C64" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update about Issue 18 and decision for variant 3
</commit_message>
<xml_diff>
--- a/0_NotesAndTesting/Test und Beispiele Indexe/Variante2_ExampleCSV.xlsx
+++ b/0_NotesAndTesting/Test und Beispiele Indexe/Variante2_ExampleCSV.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20377"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FB8632-B82B-4ED0-B203-B897FB97C3E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A7E81C-CC08-4A84-8F18-ACEFDA0B9DF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="139">
   <si>
     <t>id</t>
   </si>
@@ -355,9 +355,6 @@
     <t>Pro V2</t>
   </si>
   <si>
-    <t>//--&gt; Man kann auch beispielhaft Pfade für wiederholbare Elemente anlegen, das Konzept aufzeigen und dem Nutzer sagen er soll nach Bedarf erweitern...</t>
-  </si>
-  <si>
     <t>Kommen wirklich viele Messungen vor, die alle in die selbe Composition sollen, ist Variante 2 unumgänglich</t>
   </si>
   <si>
@@ -373,21 +370,12 @@
     <t>Erstmal Variante 1 umsetze nund später die Wahl geben, ob der Index per Hand angegeben wird oder aus einer Spalte in den Daten kommt (am Ende bei uns startend bei 0…n) ?</t>
   </si>
   <si>
-    <t>Auch noch interessant</t>
-  </si>
-  <si>
-    <t>Können wir bei V2 die notwendige CSV-Struktur aus dem Template ableiten? --&gt; ETL-Aufwand wäre dann aber das befüllen der CSV-Struktur und das Mapping würde rausfallen</t>
-  </si>
-  <si>
     <t>Contra V3</t>
   </si>
   <si>
     <t>Komplexer für den Anwender und quasi ähnlich wie V1</t>
   </si>
   <si>
-    <t>Simpel: Daten -&gt; Mapping -&gt; Pfade aus Template -&gt; Ressource</t>
-  </si>
-  <si>
     <t>Messung:1/alter</t>
   </si>
   <si>
@@ -410,6 +398,45 @@
   </si>
   <si>
     <t>Messung = 1 Item in Composition</t>
+  </si>
+  <si>
+    <t>Contra V1</t>
+  </si>
+  <si>
+    <t>Evtl. benötigte Pfade (mandatory) werden evtl. nicht gemappt</t>
+  </si>
+  <si>
+    <t>Mehrere Compositions pro Patient</t>
+  </si>
+  <si>
+    <t>Pro V3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einfache Eingabe auf CMD-Line -&gt; Nachfrage bei Nutzer   </t>
+  </si>
+  <si>
+    <t>V1 ist einfach einfach und funktioniert</t>
+  </si>
+  <si>
+    <t>Pro V1/V3</t>
+  </si>
+  <si>
+    <t>Etwas schicker für den ETLer</t>
+  </si>
+  <si>
+    <t>Fehler bei Indexierung können leicht passieren -&gt; fehlt noch ein Pfad, ist irgendwo etwas doppelt?</t>
+  </si>
+  <si>
+    <t>//--&gt; Umsetzung: Dem Nutzer verdeutlichen wie die Daten modelliert sind (Baumstruktur des WebTemplates mit Kardinalitäten in Konsole (Feature für später -&gt; für Endnutzer)</t>
+  </si>
+  <si>
+    <t>//--&gt; Abfrage der Indexe/Wiederholungen zwischen PathExport und mappingListGen</t>
+  </si>
+  <si>
+    <t>a-mpgf2</t>
+  </si>
+  <si>
+    <t>1 CSV = Daten für 1 Template</t>
   </si>
 </sst>
 </file>
@@ -440,7 +467,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -477,6 +504,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -490,7 +523,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -500,6 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -780,15 +814,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:T109"/>
+  <dimension ref="A2:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" customWidth="1"/>
@@ -806,8 +840,16 @@
     <col min="16" max="16" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
+        <v>124</v>
+      </c>
+      <c r="S3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -816,16 +858,16 @@
         <v>91</v>
       </c>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>95</v>
       </c>
       <c r="P4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="S4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -845,7 +887,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>81</v>
+        <v>137</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>82</v>
@@ -906,8 +948,8 @@
       <c r="L6" t="s">
         <v>92</v>
       </c>
-      <c r="M6" t="s">
-        <v>81</v>
+      <c r="M6" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -959,8 +1001,8 @@
       <c r="L7" t="s">
         <v>93</v>
       </c>
-      <c r="M7" t="s">
-        <v>82</v>
+      <c r="M7" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -992,10 +1034,10 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>92</v>
+        <v>4</v>
       </c>
       <c r="M8" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O8">
         <v>1</v>
@@ -1027,10 +1069,10 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>2</v>
@@ -1059,10 +1101,10 @@
         <v>4</v>
       </c>
       <c r="L10" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="M10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1072,12 +1114,6 @@
       <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="L11" t="s">
-        <v>0</v>
-      </c>
-      <c r="M11" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1090,10 +1126,7 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>94</v>
-      </c>
-      <c r="M12" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1106,52 +1139,77 @@
       <c r="C13">
         <v>0</v>
       </c>
-      <c r="L13" t="s">
-        <v>94</v>
-      </c>
-      <c r="M13" t="s">
-        <v>86</v>
-      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>99</v>
       </c>
-      <c r="L16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="E16" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
         <v>81</v>
-      </c>
-      <c r="B21" t="s">
-        <v>88</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>107</v>
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
         <v>82</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>109</v>
@@ -1160,47 +1218,47 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" t="s">
         <v>80</v>
-      </c>
-      <c r="B23" t="s">
-        <v>124</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>110</v>
       </c>
       <c r="F23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" t="s">
-        <v>123</v>
-      </c>
-      <c r="E24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>84</v>
-      </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>113</v>
-      </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1208,57 +1266,67 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B28" t="s">
-        <v>125</v>
-      </c>
-      <c r="F28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F34" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G36" t="s">
-        <v>121</v>
-      </c>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
     </row>
     <row r="43" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A43" s="8" t="s">

</xml_diff>